<commit_message>
table is creating YEEEEEEEEEEEEEAAAAAAAAAAAAAAAAAAAHHHHHH
</commit_message>
<xml_diff>
--- a/ЭДО/result.xlsx
+++ b/ЭДО/result.xlsx
@@ -52,7 +52,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -380,11 +380,81 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
@@ -535,8 +605,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="31" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="32" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -904,7 +996,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A2:AT40"/>
+  <dimension ref="A2:AT38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N36" sqref="N36"/>
@@ -1386,99 +1478,151 @@
       <c r="AP22" s="58" t="n"/>
       <c r="AQ22" s="59" t="n"/>
     </row>
-    <row r="23" ht="44.1" customHeight="1" s="12"/>
-    <row r="24" ht="6.95" customFormat="1" customHeight="1" s="4"/>
+    <row r="23" ht="50" customHeight="1" s="12">
+      <c r="B23" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" s="61" t="n"/>
+      <c r="D23" s="61" t="inlineStr">
+        <is>
+          <t>Оказание услуг по техническому обслуживанию технических средств охраны</t>
+        </is>
+      </c>
+      <c r="E23" s="61" t="n"/>
+      <c r="F23" s="61" t="n"/>
+      <c r="G23" s="61" t="n"/>
+      <c r="H23" s="61" t="n"/>
+      <c r="I23" s="61" t="n"/>
+      <c r="J23" s="61" t="n"/>
+      <c r="K23" s="61" t="n"/>
+      <c r="L23" s="61" t="n"/>
+      <c r="M23" s="61" t="n"/>
+      <c r="N23" s="61" t="n"/>
+      <c r="O23" s="61" t="n"/>
+      <c r="P23" s="61" t="n"/>
+      <c r="Q23" s="61" t="n"/>
+      <c r="R23" s="61" t="n"/>
+      <c r="S23" s="61" t="n"/>
+      <c r="T23" s="61" t="n"/>
+      <c r="U23" s="61" t="n"/>
+      <c r="V23" s="61" t="n"/>
+      <c r="W23" s="61" t="n"/>
+      <c r="X23" s="61" t="n"/>
+      <c r="Y23" s="61" t="inlineStr"/>
+      <c r="Z23" s="61" t="n"/>
+      <c r="AA23" s="61" t="n"/>
+      <c r="AB23" s="61" t="n"/>
+      <c r="AC23" s="61" t="inlineStr"/>
+      <c r="AD23" s="61" t="n"/>
+      <c r="AE23" s="61" t="n"/>
+      <c r="AF23" s="62" t="inlineStr">
+        <is>
+          <t>1812.35</t>
+        </is>
+      </c>
+      <c r="AG23" s="61" t="n"/>
+      <c r="AH23" s="61" t="n"/>
+      <c r="AI23" s="61" t="n"/>
+      <c r="AJ23" s="61" t="n"/>
+      <c r="AK23" s="62" t="inlineStr">
+        <is>
+          <t>1812.35</t>
+        </is>
+      </c>
+      <c r="AL23" s="61" t="n"/>
+      <c r="AM23" s="61" t="n"/>
+      <c r="AN23" s="61" t="n"/>
+      <c r="AO23" s="61" t="n"/>
+      <c r="AP23" s="61" t="n"/>
+      <c r="AQ23" s="63" t="n"/>
+    </row>
+    <row r="24" ht="50" customFormat="1" customHeight="1" s="4">
+      <c r="B24" s="64" t="n">
+        <v>2</v>
+      </c>
+      <c r="C24" s="61" t="n"/>
+      <c r="D24" s="61" t="inlineStr">
+        <is>
+          <t>Покупка ПК</t>
+        </is>
+      </c>
+      <c r="E24" s="61" t="n"/>
+      <c r="F24" s="61" t="n"/>
+      <c r="G24" s="61" t="n"/>
+      <c r="H24" s="61" t="n"/>
+      <c r="I24" s="61" t="n"/>
+      <c r="J24" s="61" t="n"/>
+      <c r="K24" s="61" t="n"/>
+      <c r="L24" s="61" t="n"/>
+      <c r="M24" s="61" t="n"/>
+      <c r="N24" s="61" t="n"/>
+      <c r="O24" s="61" t="n"/>
+      <c r="P24" s="61" t="n"/>
+      <c r="Q24" s="61" t="n"/>
+      <c r="R24" s="61" t="n"/>
+      <c r="S24" s="61" t="n"/>
+      <c r="T24" s="61" t="n"/>
+      <c r="U24" s="61" t="n"/>
+      <c r="V24" s="61" t="n"/>
+      <c r="W24" s="61" t="n"/>
+      <c r="X24" s="61" t="n"/>
+      <c r="Y24" s="61" t="inlineStr"/>
+      <c r="Z24" s="61" t="n"/>
+      <c r="AA24" s="61" t="n"/>
+      <c r="AB24" s="61" t="n"/>
+      <c r="AC24" s="61" t="inlineStr"/>
+      <c r="AD24" s="61" t="n"/>
+      <c r="AE24" s="61" t="n"/>
+      <c r="AF24" s="61" t="inlineStr">
+        <is>
+          <t>2000.00</t>
+        </is>
+      </c>
+      <c r="AG24" s="61" t="n"/>
+      <c r="AH24" s="61" t="n"/>
+      <c r="AI24" s="61" t="n"/>
+      <c r="AJ24" s="61" t="n"/>
+      <c r="AK24" s="61" t="inlineStr">
+        <is>
+          <t>2000.00</t>
+        </is>
+      </c>
+      <c r="AL24" s="61" t="n"/>
+      <c r="AM24" s="61" t="n"/>
+      <c r="AN24" s="61" t="n"/>
+      <c r="AO24" s="61" t="n"/>
+      <c r="AP24" s="61" t="n"/>
+      <c r="AQ24" s="63" t="n"/>
+    </row>
     <row r="25" ht="12.95" customHeight="1" s="12">
-      <c r="B25" s="39" t="n">
-        <v>1</v>
-      </c>
-      <c r="C25" s="60" t="n"/>
-      <c r="D25" s="40" t="n"/>
-      <c r="E25" s="60" t="n"/>
-      <c r="F25" s="60" t="n"/>
-      <c r="G25" s="60" t="n"/>
-      <c r="H25" s="60" t="n"/>
-      <c r="I25" s="60" t="n"/>
-      <c r="J25" s="60" t="n"/>
-      <c r="K25" s="60" t="n"/>
-      <c r="L25" s="60" t="n"/>
-      <c r="M25" s="60" t="n"/>
-      <c r="N25" s="60" t="n"/>
-      <c r="O25" s="60" t="n"/>
-      <c r="P25" s="60" t="n"/>
-      <c r="Q25" s="60" t="n"/>
-      <c r="R25" s="60" t="n"/>
-      <c r="S25" s="60" t="n"/>
-      <c r="T25" s="60" t="n"/>
-      <c r="U25" s="60" t="n"/>
-      <c r="V25" s="60" t="n"/>
-      <c r="W25" s="60" t="n"/>
-      <c r="X25" s="60" t="n"/>
-      <c r="Y25" s="5" t="n"/>
-      <c r="Z25" s="6" t="n"/>
-      <c r="AA25" s="6" t="n"/>
-      <c r="AB25" s="6" t="n"/>
-      <c r="AC25" s="7" t="n"/>
-      <c r="AD25" s="8" t="n"/>
-      <c r="AE25" s="8" t="n"/>
-      <c r="AF25" s="41" t="n"/>
-      <c r="AG25" s="60" t="n"/>
-      <c r="AH25" s="60" t="n"/>
-      <c r="AI25" s="60" t="n"/>
-      <c r="AJ25" s="60" t="n"/>
-      <c r="AK25" s="42" t="n"/>
-      <c r="AL25" s="60" t="n"/>
-      <c r="AM25" s="60" t="n"/>
-      <c r="AN25" s="60" t="n"/>
-      <c r="AO25" s="60" t="n"/>
-      <c r="AP25" s="60" t="n"/>
-      <c r="AQ25" s="61" t="n"/>
+      <c r="AA25" s="2" t="n"/>
+      <c r="AB25" s="2" t="n"/>
+      <c r="AC25" s="2" t="n"/>
+      <c r="AD25" s="2" t="n"/>
+      <c r="AE25" s="2" t="n"/>
+      <c r="AF25" s="2" t="n"/>
+      <c r="AG25" s="2" t="n"/>
+      <c r="AH25" s="2" t="n"/>
+      <c r="AI25" s="2" t="n"/>
+      <c r="AJ25" s="2" t="n"/>
+      <c r="AK25" s="2" t="n"/>
+      <c r="AL25" s="37" t="n"/>
     </row>
     <row r="26" ht="12.95" customHeight="1" s="12">
-      <c r="B26" s="4" t="n"/>
-      <c r="C26" s="4" t="n"/>
-      <c r="D26" s="4" t="n"/>
-      <c r="E26" s="4" t="n"/>
-      <c r="F26" s="4" t="n"/>
-      <c r="G26" s="4" t="n"/>
-      <c r="H26" s="4" t="n"/>
-      <c r="I26" s="4" t="n"/>
-      <c r="J26" s="4" t="n"/>
-      <c r="K26" s="4" t="n"/>
-      <c r="L26" s="4" t="n"/>
-      <c r="M26" s="4" t="n"/>
-      <c r="N26" s="4" t="n"/>
-      <c r="O26" s="4" t="n"/>
-      <c r="P26" s="4" t="n"/>
-      <c r="Q26" s="4" t="n"/>
-      <c r="R26" s="4" t="n"/>
-      <c r="S26" s="4" t="n"/>
-      <c r="T26" s="4" t="n"/>
-      <c r="U26" s="4" t="n"/>
-      <c r="V26" s="4" t="n"/>
-      <c r="W26" s="4" t="n"/>
-      <c r="X26" s="4" t="n"/>
-      <c r="Y26" s="4" t="n"/>
-      <c r="Z26" s="4" t="n"/>
-      <c r="AA26" s="4" t="n"/>
-      <c r="AB26" s="4" t="n"/>
-      <c r="AC26" s="4" t="n"/>
-      <c r="AD26" s="4" t="n"/>
-      <c r="AE26" s="4" t="n"/>
-      <c r="AF26" s="4" t="n"/>
-      <c r="AG26" s="4" t="n"/>
-      <c r="AH26" s="4" t="n"/>
-      <c r="AI26" s="4" t="n"/>
-      <c r="AJ26" s="4" t="n"/>
-      <c r="AK26" s="4" t="n"/>
-      <c r="AL26" s="4" t="n"/>
-      <c r="AM26" s="4" t="n"/>
-      <c r="AN26" s="4" t="n"/>
-      <c r="AO26" s="4" t="n"/>
-      <c r="AP26" s="4" t="n"/>
-      <c r="AQ26" s="4" t="n"/>
-    </row>
-    <row r="27" ht="12.95" customHeight="1" s="12">
+      <c r="AA26" s="2" t="n"/>
+      <c r="AB26" s="2" t="n"/>
+      <c r="AC26" s="2" t="n"/>
+      <c r="AD26" s="2" t="n"/>
+      <c r="AE26" s="2" t="n"/>
+      <c r="AF26" s="2" t="n"/>
+      <c r="AG26" s="2" t="n"/>
+      <c r="AH26" s="2" t="n"/>
+      <c r="AI26" s="2" t="n"/>
+      <c r="AJ26" s="2" t="n"/>
+      <c r="AK26" s="2" t="n"/>
+      <c r="AL26" s="37" t="n"/>
+    </row>
+    <row r="27" ht="15" customHeight="1" s="12">
       <c r="AA27" s="2" t="n"/>
       <c r="AB27" s="2" t="n"/>
       <c r="AC27" s="2" t="n"/>
@@ -1489,126 +1633,183 @@
       <c r="AH27" s="2" t="n"/>
       <c r="AI27" s="2" t="n"/>
       <c r="AJ27" s="2" t="n"/>
-      <c r="AK27" s="2" t="n"/>
-      <c r="AL27" s="37" t="n"/>
-    </row>
-    <row r="28" ht="12.95" customHeight="1" s="12">
-      <c r="AA28" s="2" t="n"/>
-      <c r="AB28" s="2" t="n"/>
-      <c r="AC28" s="2" t="n"/>
-      <c r="AD28" s="2" t="n"/>
-      <c r="AE28" s="2" t="n"/>
-      <c r="AF28" s="2" t="n"/>
-      <c r="AG28" s="2" t="n"/>
-      <c r="AH28" s="2" t="n"/>
-      <c r="AI28" s="2" t="n"/>
-      <c r="AJ28" s="2" t="n"/>
-      <c r="AK28" s="2" t="n"/>
-      <c r="AL28" s="37" t="n"/>
-    </row>
-    <row r="29" ht="12.95" customHeight="1" s="12">
-      <c r="AA29" s="2" t="n"/>
-      <c r="AB29" s="2" t="n"/>
-      <c r="AC29" s="2" t="n"/>
-      <c r="AD29" s="2" t="n"/>
-      <c r="AE29" s="2" t="n"/>
-      <c r="AF29" s="2" t="n"/>
-      <c r="AG29" s="2" t="n"/>
-      <c r="AH29" s="2" t="n"/>
-      <c r="AI29" s="2" t="n"/>
-      <c r="AJ29" s="2" t="n"/>
-      <c r="AK29" s="2" t="n"/>
-      <c r="AL29" s="37" t="n"/>
-    </row>
-    <row r="30" ht="6.95" customFormat="1" customHeight="1" s="4">
-      <c r="B30" s="9" t="n"/>
-      <c r="C30" s="9" t="n"/>
-      <c r="D30" s="9" t="n"/>
-      <c r="E30" s="9" t="n"/>
-      <c r="F30" s="9" t="n"/>
-      <c r="G30" s="9" t="n"/>
-      <c r="H30" s="9" t="n"/>
-      <c r="I30" s="9" t="n"/>
-      <c r="J30" s="9" t="n"/>
-      <c r="K30" s="9" t="n"/>
-      <c r="L30" s="9" t="n"/>
-      <c r="M30" s="9" t="n"/>
-      <c r="N30" s="9" t="n"/>
-      <c r="O30" s="9" t="n"/>
-      <c r="P30" s="9" t="n"/>
-      <c r="Q30" s="9" t="n"/>
-      <c r="R30" s="9" t="n"/>
-      <c r="S30" s="9" t="n"/>
-      <c r="T30" s="9" t="n"/>
-      <c r="U30" s="9" t="n"/>
-      <c r="V30" s="9" t="n"/>
-      <c r="W30" s="9" t="n"/>
-      <c r="X30" s="9" t="n"/>
-      <c r="Y30" s="9" t="n"/>
-      <c r="Z30" s="9" t="n"/>
-      <c r="AA30" s="9" t="n"/>
-      <c r="AB30" s="9" t="n"/>
-      <c r="AC30" s="9" t="n"/>
-      <c r="AD30" s="9" t="n"/>
-      <c r="AE30" s="9" t="n"/>
-      <c r="AF30" s="9" t="n"/>
-      <c r="AG30" s="9" t="n"/>
-      <c r="AH30" s="9" t="n"/>
-      <c r="AI30" s="9" t="n"/>
-      <c r="AJ30" s="9" t="n"/>
-      <c r="AK30" s="9" t="n"/>
-      <c r="AL30" s="9" t="n"/>
-      <c r="AM30" s="9" t="n"/>
-      <c r="AN30" s="9" t="n"/>
-      <c r="AO30" s="9" t="n"/>
-      <c r="AP30" s="9" t="n"/>
-      <c r="AQ30" s="9" t="n"/>
-      <c r="AR30" s="9" t="n"/>
-    </row>
+      <c r="AK27" s="65" t="inlineStr">
+        <is>
+          <t>Итого:</t>
+        </is>
+      </c>
+      <c r="AL27" s="66" t="n"/>
+    </row>
+    <row r="28" ht="15" customHeight="1" s="12">
+      <c r="B28" s="9" t="n"/>
+      <c r="C28" s="9" t="n"/>
+      <c r="D28" s="9" t="n"/>
+      <c r="E28" s="9" t="n"/>
+      <c r="F28" s="9" t="n"/>
+      <c r="G28" s="9" t="n"/>
+      <c r="H28" s="9" t="n"/>
+      <c r="I28" s="9" t="n"/>
+      <c r="J28" s="9" t="n"/>
+      <c r="K28" s="9" t="n"/>
+      <c r="L28" s="9" t="n"/>
+      <c r="M28" s="9" t="n"/>
+      <c r="N28" s="9" t="n"/>
+      <c r="O28" s="9" t="n"/>
+      <c r="P28" s="9" t="n"/>
+      <c r="Q28" s="9" t="n"/>
+      <c r="R28" s="9" t="n"/>
+      <c r="S28" s="9" t="n"/>
+      <c r="T28" s="9" t="n"/>
+      <c r="U28" s="9" t="n"/>
+      <c r="V28" s="9" t="n"/>
+      <c r="W28" s="9" t="n"/>
+      <c r="X28" s="9" t="n"/>
+      <c r="Y28" s="9" t="n"/>
+      <c r="Z28" s="9" t="n"/>
+      <c r="AA28" s="9" t="n"/>
+      <c r="AB28" s="9" t="n"/>
+      <c r="AC28" s="9" t="n"/>
+      <c r="AD28" s="9" t="n"/>
+      <c r="AE28" s="9" t="n"/>
+      <c r="AF28" s="9" t="n"/>
+      <c r="AG28" s="9" t="n"/>
+      <c r="AH28" s="9" t="n"/>
+      <c r="AI28" s="9" t="n"/>
+      <c r="AJ28" s="9" t="n"/>
+      <c r="AK28" s="67" t="n"/>
+      <c r="AL28" s="67" t="n"/>
+      <c r="AR28" s="9" t="n"/>
+    </row>
+    <row r="29" ht="15" customHeight="1" s="12">
+      <c r="B29" s="10" t="n"/>
+      <c r="C29" s="10" t="n"/>
+      <c r="D29" s="10" t="n"/>
+      <c r="E29" s="10" t="n"/>
+      <c r="F29" s="10" t="n"/>
+      <c r="G29" s="10" t="n"/>
+      <c r="H29" s="10" t="n"/>
+      <c r="I29" s="10" t="n"/>
+      <c r="J29" s="10" t="n"/>
+      <c r="K29" s="10" t="n"/>
+      <c r="L29" s="10" t="n"/>
+      <c r="M29" s="10" t="n"/>
+      <c r="N29" s="10" t="n"/>
+      <c r="O29" s="10" t="n"/>
+      <c r="P29" s="10" t="n"/>
+      <c r="Q29" s="10" t="n"/>
+      <c r="R29" s="10" t="n"/>
+      <c r="S29" s="10" t="n"/>
+      <c r="T29" s="10" t="n"/>
+      <c r="U29" s="10" t="n"/>
+      <c r="V29" s="10" t="n"/>
+      <c r="W29" s="10" t="n"/>
+      <c r="X29" s="10" t="n"/>
+      <c r="Y29" s="10" t="n"/>
+      <c r="Z29" s="10" t="n"/>
+      <c r="AA29" s="10" t="n"/>
+      <c r="AB29" s="10" t="n"/>
+      <c r="AC29" s="10" t="n"/>
+      <c r="AD29" s="10" t="n"/>
+      <c r="AE29" s="10" t="n"/>
+      <c r="AF29" s="10" t="n"/>
+      <c r="AG29" s="10" t="n"/>
+      <c r="AH29" s="10" t="n"/>
+      <c r="AI29" s="10" t="n"/>
+      <c r="AJ29" s="10" t="n"/>
+      <c r="AK29" s="65" t="n"/>
+      <c r="AL29" s="65" t="n"/>
+    </row>
+    <row r="30" ht="6.95" customFormat="1" customHeight="1" s="4"/>
     <row r="31" ht="12" customFormat="1" customHeight="1" s="4">
-      <c r="B31" s="10" t="n"/>
-      <c r="C31" s="10" t="n"/>
-      <c r="D31" s="10" t="n"/>
-      <c r="E31" s="10" t="n"/>
-      <c r="F31" s="10" t="n"/>
-      <c r="G31" s="10" t="n"/>
-      <c r="H31" s="10" t="n"/>
-      <c r="I31" s="10" t="n"/>
-      <c r="J31" s="10" t="n"/>
-      <c r="K31" s="10" t="n"/>
-      <c r="L31" s="10" t="n"/>
-      <c r="M31" s="10" t="n"/>
-      <c r="N31" s="10" t="n"/>
-      <c r="O31" s="10" t="n"/>
-      <c r="P31" s="10" t="n"/>
-      <c r="Q31" s="10" t="n"/>
-      <c r="R31" s="10" t="n"/>
-      <c r="S31" s="10" t="n"/>
-      <c r="T31" s="10" t="n"/>
-      <c r="U31" s="10" t="n"/>
-      <c r="V31" s="10" t="n"/>
-      <c r="W31" s="10" t="n"/>
-      <c r="X31" s="10" t="n"/>
-      <c r="Y31" s="10" t="n"/>
-      <c r="Z31" s="10" t="n"/>
-      <c r="AA31" s="10" t="n"/>
-      <c r="AB31" s="10" t="n"/>
-      <c r="AC31" s="10" t="n"/>
-      <c r="AD31" s="10" t="n"/>
-      <c r="AE31" s="10" t="n"/>
-      <c r="AF31" s="10" t="n"/>
-      <c r="AG31" s="10" t="n"/>
-      <c r="AH31" s="10" t="n"/>
-      <c r="AI31" s="10" t="n"/>
-      <c r="AJ31" s="10" t="n"/>
-      <c r="AK31" s="10" t="n"/>
-      <c r="AL31" s="10" t="n"/>
-      <c r="AM31" s="10" t="n"/>
-      <c r="AN31" s="10" t="n"/>
-      <c r="AO31" s="10" t="n"/>
-      <c r="AP31" s="10" t="n"/>
-    </row>
-    <row r="32" ht="12" customFormat="1" customHeight="1" s="4"/>
+      <c r="B31" s="11" t="n"/>
+      <c r="C31" s="11" t="n"/>
+      <c r="D31" s="11" t="n"/>
+      <c r="E31" s="11" t="n"/>
+      <c r="F31" s="11" t="n"/>
+      <c r="G31" s="11" t="n"/>
+      <c r="H31" s="11" t="n"/>
+      <c r="I31" s="11" t="n"/>
+      <c r="J31" s="11" t="n"/>
+      <c r="K31" s="11" t="n"/>
+      <c r="L31" s="11" t="n"/>
+      <c r="M31" s="11" t="n"/>
+      <c r="N31" s="11" t="n"/>
+      <c r="O31" s="11" t="n"/>
+      <c r="P31" s="11" t="n"/>
+      <c r="Q31" s="11" t="n"/>
+      <c r="R31" s="11" t="n"/>
+      <c r="S31" s="11" t="n"/>
+      <c r="T31" s="11" t="n"/>
+      <c r="U31" s="11" t="n"/>
+      <c r="V31" s="11" t="n"/>
+      <c r="W31" s="11" t="n"/>
+      <c r="X31" s="11" t="n"/>
+      <c r="Y31" s="11" t="n"/>
+      <c r="Z31" s="11" t="n"/>
+      <c r="AA31" s="11" t="n"/>
+      <c r="AB31" s="11" t="n"/>
+      <c r="AC31" s="11" t="n"/>
+      <c r="AD31" s="11" t="n"/>
+      <c r="AE31" s="11" t="n"/>
+      <c r="AF31" s="11" t="n"/>
+      <c r="AG31" s="11" t="n"/>
+      <c r="AH31" s="11" t="n"/>
+      <c r="AI31" s="11" t="n"/>
+      <c r="AJ31" s="11" t="n"/>
+      <c r="AK31" s="11" t="n"/>
+      <c r="AL31" s="11" t="n"/>
+      <c r="AM31" s="11" t="n"/>
+      <c r="AN31" s="11" t="n"/>
+      <c r="AO31" s="11" t="n"/>
+      <c r="AP31" s="11" t="n"/>
+      <c r="AQ31" s="11" t="n"/>
+      <c r="AR31" s="11" t="n"/>
+    </row>
+    <row r="32" ht="12" customFormat="1" customHeight="1" s="4">
+      <c r="B32" s="11" t="n"/>
+      <c r="C32" s="11" t="n"/>
+      <c r="D32" s="11" t="n"/>
+      <c r="E32" s="11" t="n"/>
+      <c r="F32" s="11" t="n"/>
+      <c r="G32" s="11" t="n"/>
+      <c r="H32" s="11" t="n"/>
+      <c r="I32" s="11" t="n"/>
+      <c r="J32" s="11" t="n"/>
+      <c r="K32" s="11" t="n"/>
+      <c r="L32" s="11" t="n"/>
+      <c r="M32" s="11" t="n"/>
+      <c r="N32" s="11" t="n"/>
+      <c r="O32" s="11" t="n"/>
+      <c r="P32" s="11" t="n"/>
+      <c r="Q32" s="11" t="n"/>
+      <c r="R32" s="11" t="n"/>
+      <c r="S32" s="11" t="n"/>
+      <c r="T32" s="11" t="n"/>
+      <c r="U32" s="11" t="n"/>
+      <c r="V32" s="11" t="n"/>
+      <c r="W32" s="11" t="n"/>
+      <c r="X32" s="11" t="n"/>
+      <c r="Y32" s="11" t="n"/>
+      <c r="Z32" s="11" t="n"/>
+      <c r="AA32" s="11" t="n"/>
+      <c r="AB32" s="11" t="n"/>
+      <c r="AC32" s="11" t="n"/>
+      <c r="AD32" s="11" t="n"/>
+      <c r="AE32" s="11" t="n"/>
+      <c r="AF32" s="11" t="n"/>
+      <c r="AG32" s="11" t="n"/>
+      <c r="AH32" s="11" t="n"/>
+      <c r="AI32" s="11" t="n"/>
+      <c r="AJ32" s="11" t="n"/>
+      <c r="AK32" s="11" t="n"/>
+      <c r="AL32" s="11" t="n"/>
+      <c r="AM32" s="11" t="n"/>
+      <c r="AN32" s="11" t="n"/>
+      <c r="AO32" s="11" t="n"/>
+      <c r="AP32" s="11" t="n"/>
+      <c r="AQ32" s="11" t="n"/>
+      <c r="AR32" s="11" t="n"/>
+    </row>
     <row r="33" ht="12" customFormat="1" customHeight="1" s="4">
       <c r="B33" s="11" t="n"/>
       <c r="C33" s="11" t="n"/>
@@ -1655,6 +1856,7 @@
       <c r="AR33" s="11" t="n"/>
     </row>
     <row r="34" ht="9.75" customFormat="1" customHeight="1" s="4">
+      <c r="A34" s="4" t="n"/>
       <c r="B34" s="11" t="n"/>
       <c r="C34" s="11" t="n"/>
       <c r="D34" s="11" t="n"/>
@@ -1698,103 +1900,107 @@
       <c r="AP34" s="11" t="n"/>
       <c r="AQ34" s="11" t="n"/>
       <c r="AR34" s="11" t="n"/>
+      <c r="AS34" s="4" t="n"/>
+      <c r="AT34" s="4" t="n"/>
     </row>
     <row r="35" ht="6.95" customFormat="1" customHeight="1" s="4">
-      <c r="B35" s="11" t="n"/>
-      <c r="C35" s="11" t="n"/>
-      <c r="D35" s="11" t="n"/>
-      <c r="E35" s="11" t="n"/>
-      <c r="F35" s="11" t="n"/>
-      <c r="G35" s="11" t="n"/>
-      <c r="H35" s="11" t="n"/>
-      <c r="I35" s="11" t="n"/>
-      <c r="J35" s="11" t="n"/>
-      <c r="K35" s="11" t="n"/>
-      <c r="L35" s="11" t="n"/>
-      <c r="M35" s="11" t="n"/>
-      <c r="N35" s="11" t="n"/>
-      <c r="O35" s="11" t="n"/>
-      <c r="P35" s="11" t="n"/>
-      <c r="Q35" s="11" t="n"/>
-      <c r="R35" s="11" t="n"/>
-      <c r="S35" s="11" t="n"/>
-      <c r="T35" s="11" t="n"/>
-      <c r="U35" s="11" t="n"/>
-      <c r="V35" s="11" t="n"/>
-      <c r="W35" s="11" t="n"/>
-      <c r="X35" s="11" t="n"/>
-      <c r="Y35" s="11" t="n"/>
-      <c r="Z35" s="11" t="n"/>
-      <c r="AA35" s="11" t="n"/>
-      <c r="AB35" s="11" t="n"/>
-      <c r="AC35" s="11" t="n"/>
-      <c r="AD35" s="11" t="n"/>
-      <c r="AE35" s="11" t="n"/>
-      <c r="AF35" s="11" t="n"/>
-      <c r="AG35" s="11" t="n"/>
-      <c r="AH35" s="11" t="n"/>
-      <c r="AI35" s="11" t="n"/>
-      <c r="AJ35" s="11" t="n"/>
-      <c r="AK35" s="11" t="n"/>
-      <c r="AL35" s="11" t="n"/>
-      <c r="AM35" s="11" t="n"/>
-      <c r="AN35" s="11" t="n"/>
-      <c r="AO35" s="11" t="n"/>
-      <c r="AP35" s="11" t="n"/>
-      <c r="AQ35" s="11" t="n"/>
-      <c r="AR35" s="11" t="n"/>
+      <c r="A35" s="4" t="n"/>
+      <c r="B35" s="4" t="n"/>
+      <c r="C35" s="4" t="n"/>
+      <c r="D35" s="4" t="n"/>
+      <c r="E35" s="4" t="n"/>
+      <c r="F35" s="4" t="n"/>
+      <c r="G35" s="4" t="n"/>
+      <c r="H35" s="4" t="n"/>
+      <c r="I35" s="4" t="n"/>
+      <c r="J35" s="4" t="n"/>
+      <c r="K35" s="4" t="n"/>
+      <c r="L35" s="4" t="n"/>
+      <c r="M35" s="4" t="n"/>
+      <c r="N35" s="4" t="n"/>
+      <c r="O35" s="4" t="n"/>
+      <c r="P35" s="4" t="n"/>
+      <c r="Q35" s="4" t="n"/>
+      <c r="R35" s="4" t="n"/>
+      <c r="S35" s="4" t="n"/>
+      <c r="T35" s="4" t="n"/>
+      <c r="U35" s="4" t="n"/>
+      <c r="V35" s="4" t="n"/>
+      <c r="W35" s="4" t="n"/>
+      <c r="X35" s="4" t="n"/>
+      <c r="Y35" s="4" t="n"/>
+      <c r="Z35" s="4" t="n"/>
+      <c r="AA35" s="4" t="n"/>
+      <c r="AB35" s="4" t="n"/>
+      <c r="AC35" s="4" t="n"/>
+      <c r="AD35" s="4" t="n"/>
+      <c r="AE35" s="4" t="n"/>
+      <c r="AF35" s="4" t="n"/>
+      <c r="AG35" s="4" t="n"/>
+      <c r="AH35" s="4" t="n"/>
+      <c r="AI35" s="4" t="n"/>
+      <c r="AJ35" s="4" t="n"/>
+      <c r="AK35" s="4" t="n"/>
+      <c r="AL35" s="4" t="n"/>
+      <c r="AM35" s="4" t="n"/>
+      <c r="AN35" s="4" t="n"/>
+      <c r="AO35" s="4" t="n"/>
+      <c r="AP35" s="4" t="n"/>
+      <c r="AQ35" s="4" t="n"/>
+      <c r="AR35" s="4" t="n"/>
+      <c r="AS35" s="4" t="n"/>
+      <c r="AT35" s="4" t="n"/>
     </row>
     <row r="36" ht="11.45" customHeight="1" s="12">
       <c r="A36" s="4" t="n"/>
-      <c r="B36" s="11" t="n"/>
-      <c r="C36" s="11" t="n"/>
-      <c r="D36" s="11" t="n"/>
-      <c r="E36" s="11" t="n"/>
-      <c r="F36" s="11" t="n"/>
-      <c r="G36" s="11" t="n"/>
-      <c r="H36" s="11" t="n"/>
-      <c r="I36" s="11" t="n"/>
-      <c r="J36" s="11" t="n"/>
-      <c r="K36" s="11" t="n"/>
-      <c r="L36" s="11" t="n"/>
-      <c r="M36" s="11" t="n"/>
-      <c r="N36" s="11" t="n"/>
-      <c r="O36" s="11" t="n"/>
-      <c r="P36" s="11" t="n"/>
-      <c r="Q36" s="11" t="n"/>
-      <c r="R36" s="11" t="n"/>
-      <c r="S36" s="11" t="n"/>
-      <c r="T36" s="11" t="n"/>
-      <c r="U36" s="11" t="n"/>
-      <c r="V36" s="11" t="n"/>
-      <c r="W36" s="11" t="n"/>
-      <c r="X36" s="11" t="n"/>
-      <c r="Y36" s="11" t="n"/>
-      <c r="Z36" s="11" t="n"/>
-      <c r="AA36" s="11" t="n"/>
-      <c r="AB36" s="11" t="n"/>
-      <c r="AC36" s="11" t="n"/>
-      <c r="AD36" s="11" t="n"/>
-      <c r="AE36" s="11" t="n"/>
-      <c r="AF36" s="11" t="n"/>
-      <c r="AG36" s="11" t="n"/>
-      <c r="AH36" s="11" t="n"/>
-      <c r="AI36" s="11" t="n"/>
-      <c r="AJ36" s="11" t="n"/>
-      <c r="AK36" s="11" t="n"/>
-      <c r="AL36" s="11" t="n"/>
-      <c r="AM36" s="11" t="n"/>
-      <c r="AN36" s="11" t="n"/>
-      <c r="AO36" s="11" t="n"/>
-      <c r="AP36" s="11" t="n"/>
-      <c r="AQ36" s="11" t="n"/>
-      <c r="AR36" s="11" t="n"/>
+      <c r="B36" s="4" t="n"/>
+      <c r="C36" s="4" t="n"/>
+      <c r="D36" s="4" t="n"/>
+      <c r="E36" s="4" t="n"/>
+      <c r="F36" s="4" t="n"/>
+      <c r="G36" s="4" t="n"/>
+      <c r="H36" s="4" t="n"/>
+      <c r="I36" s="4" t="n"/>
+      <c r="J36" s="4" t="n"/>
+      <c r="K36" s="4" t="n"/>
+      <c r="L36" s="4" t="n"/>
+      <c r="M36" s="4" t="n"/>
+      <c r="N36" s="4" t="n"/>
+      <c r="O36" s="4" t="n"/>
+      <c r="P36" s="4" t="n"/>
+      <c r="Q36" s="4" t="n"/>
+      <c r="R36" s="4" t="n"/>
+      <c r="S36" s="4" t="n"/>
+      <c r="T36" s="4" t="n"/>
+      <c r="U36" s="4" t="n"/>
+      <c r="V36" s="4" t="n"/>
+      <c r="W36" s="4" t="n"/>
+      <c r="X36" s="4" t="n"/>
+      <c r="Y36" s="4" t="n"/>
+      <c r="Z36" s="4" t="n"/>
+      <c r="AA36" s="4" t="n"/>
+      <c r="AB36" s="4" t="n"/>
+      <c r="AC36" s="4" t="n"/>
+      <c r="AD36" s="4" t="n"/>
+      <c r="AE36" s="4" t="n"/>
+      <c r="AF36" s="4" t="n"/>
+      <c r="AG36" s="4" t="n"/>
+      <c r="AH36" s="4" t="n"/>
+      <c r="AI36" s="4" t="n"/>
+      <c r="AJ36" s="4" t="n"/>
+      <c r="AK36" s="4" t="n"/>
+      <c r="AL36" s="4" t="n"/>
+      <c r="AM36" s="4" t="n"/>
+      <c r="AN36" s="4" t="n"/>
+      <c r="AO36" s="4" t="n"/>
+      <c r="AP36" s="4" t="n"/>
+      <c r="AQ36" s="4" t="n"/>
+      <c r="AR36" s="4" t="n"/>
       <c r="AS36" s="4" t="n"/>
-      <c r="AT36" s="4" t="n"/>
     </row>
     <row r="37" ht="12.95" customHeight="1" s="12">
       <c r="A37" s="4" t="n"/>
-      <c r="B37" s="4" t="n"/>
+      <c r="B37" s="13" t="n"/>
       <c r="C37" s="4" t="n"/>
       <c r="D37" s="4" t="n"/>
       <c r="E37" s="4" t="n"/>
@@ -1805,21 +2011,21 @@
       <c r="J37" s="4" t="n"/>
       <c r="K37" s="4" t="n"/>
       <c r="L37" s="4" t="n"/>
-      <c r="M37" s="4" t="n"/>
-      <c r="N37" s="4" t="n"/>
-      <c r="O37" s="4" t="n"/>
-      <c r="P37" s="4" t="n"/>
-      <c r="Q37" s="4" t="n"/>
-      <c r="R37" s="4" t="n"/>
-      <c r="S37" s="4" t="n"/>
-      <c r="T37" s="4" t="n"/>
-      <c r="U37" s="4" t="n"/>
-      <c r="V37" s="4" t="n"/>
-      <c r="W37" s="4" t="n"/>
+      <c r="M37" s="14" t="n"/>
+      <c r="N37" s="14" t="n"/>
+      <c r="O37" s="14" t="n"/>
+      <c r="P37" s="14" t="n"/>
+      <c r="Q37" s="14" t="n"/>
+      <c r="R37" s="14" t="n"/>
+      <c r="S37" s="14" t="n"/>
+      <c r="T37" s="14" t="n"/>
+      <c r="U37" s="14" t="n"/>
+      <c r="V37" s="14" t="n"/>
+      <c r="W37" s="14" t="n"/>
       <c r="X37" s="4" t="n"/>
       <c r="Y37" s="4" t="n"/>
-      <c r="Z37" s="4" t="n"/>
-      <c r="AA37" s="4" t="n"/>
+      <c r="Z37" s="13" t="n"/>
+      <c r="AA37" s="13" t="n"/>
       <c r="AB37" s="4" t="n"/>
       <c r="AC37" s="4" t="n"/>
       <c r="AD37" s="4" t="n"/>
@@ -1828,17 +2034,16 @@
       <c r="AG37" s="4" t="n"/>
       <c r="AH37" s="4" t="n"/>
       <c r="AI37" s="4" t="n"/>
-      <c r="AJ37" s="4" t="n"/>
-      <c r="AK37" s="4" t="n"/>
-      <c r="AL37" s="4" t="n"/>
-      <c r="AM37" s="4" t="n"/>
-      <c r="AN37" s="4" t="n"/>
-      <c r="AO37" s="4" t="n"/>
-      <c r="AP37" s="4" t="n"/>
-      <c r="AQ37" s="4" t="n"/>
-      <c r="AR37" s="4" t="n"/>
+      <c r="AJ37" s="14" t="n"/>
+      <c r="AK37" s="14" t="n"/>
+      <c r="AL37" s="14" t="n"/>
+      <c r="AM37" s="14" t="n"/>
+      <c r="AN37" s="14" t="n"/>
+      <c r="AO37" s="14" t="n"/>
+      <c r="AP37" s="14" t="n"/>
+      <c r="AQ37" s="14" t="n"/>
+      <c r="AR37" s="14" t="n"/>
       <c r="AS37" s="4" t="n"/>
-      <c r="AT37" s="4" t="n"/>
     </row>
     <row r="38" ht="11.1" customHeight="1" s="12">
       <c r="A38" s="4" t="n"/>
@@ -1887,102 +2092,8 @@
       <c r="AR38" s="4" t="n"/>
       <c r="AS38" s="4" t="n"/>
     </row>
-    <row r="39">
-      <c r="A39" s="4" t="n"/>
-      <c r="B39" s="13" t="n"/>
-      <c r="C39" s="4" t="n"/>
-      <c r="D39" s="4" t="n"/>
-      <c r="E39" s="4" t="n"/>
-      <c r="F39" s="4" t="n"/>
-      <c r="G39" s="4" t="n"/>
-      <c r="H39" s="4" t="n"/>
-      <c r="I39" s="4" t="n"/>
-      <c r="J39" s="4" t="n"/>
-      <c r="K39" s="4" t="n"/>
-      <c r="L39" s="4" t="n"/>
-      <c r="M39" s="14" t="n"/>
-      <c r="N39" s="14" t="n"/>
-      <c r="O39" s="14" t="n"/>
-      <c r="P39" s="14" t="n"/>
-      <c r="Q39" s="14" t="n"/>
-      <c r="R39" s="14" t="n"/>
-      <c r="S39" s="14" t="n"/>
-      <c r="T39" s="14" t="n"/>
-      <c r="U39" s="14" t="n"/>
-      <c r="V39" s="14" t="n"/>
-      <c r="W39" s="14" t="n"/>
-      <c r="X39" s="4" t="n"/>
-      <c r="Y39" s="4" t="n"/>
-      <c r="Z39" s="13" t="n"/>
-      <c r="AA39" s="13" t="n"/>
-      <c r="AB39" s="4" t="n"/>
-      <c r="AC39" s="4" t="n"/>
-      <c r="AD39" s="4" t="n"/>
-      <c r="AE39" s="4" t="n"/>
-      <c r="AF39" s="4" t="n"/>
-      <c r="AG39" s="4" t="n"/>
-      <c r="AH39" s="4" t="n"/>
-      <c r="AI39" s="4" t="n"/>
-      <c r="AJ39" s="14" t="n"/>
-      <c r="AK39" s="14" t="n"/>
-      <c r="AL39" s="14" t="n"/>
-      <c r="AM39" s="14" t="n"/>
-      <c r="AN39" s="14" t="n"/>
-      <c r="AO39" s="14" t="n"/>
-      <c r="AP39" s="14" t="n"/>
-      <c r="AQ39" s="14" t="n"/>
-      <c r="AR39" s="14" t="n"/>
-      <c r="AS39" s="4" t="n"/>
-    </row>
-    <row r="40">
-      <c r="A40" s="4" t="n"/>
-      <c r="B40" s="4" t="n"/>
-      <c r="C40" s="4" t="n"/>
-      <c r="D40" s="4" t="n"/>
-      <c r="E40" s="4" t="n"/>
-      <c r="F40" s="4" t="n"/>
-      <c r="G40" s="4" t="n"/>
-      <c r="H40" s="4" t="n"/>
-      <c r="I40" s="4" t="n"/>
-      <c r="J40" s="4" t="n"/>
-      <c r="K40" s="4" t="n"/>
-      <c r="L40" s="4" t="n"/>
-      <c r="M40" s="4" t="n"/>
-      <c r="N40" s="4" t="n"/>
-      <c r="O40" s="4" t="n"/>
-      <c r="P40" s="4" t="n"/>
-      <c r="Q40" s="4" t="n"/>
-      <c r="R40" s="4" t="n"/>
-      <c r="S40" s="4" t="n"/>
-      <c r="T40" s="4" t="n"/>
-      <c r="U40" s="4" t="n"/>
-      <c r="V40" s="4" t="n"/>
-      <c r="W40" s="4" t="n"/>
-      <c r="X40" s="4" t="n"/>
-      <c r="Y40" s="4" t="n"/>
-      <c r="Z40" s="4" t="n"/>
-      <c r="AA40" s="4" t="n"/>
-      <c r="AB40" s="4" t="n"/>
-      <c r="AC40" s="4" t="n"/>
-      <c r="AD40" s="4" t="n"/>
-      <c r="AE40" s="4" t="n"/>
-      <c r="AF40" s="4" t="n"/>
-      <c r="AG40" s="4" t="n"/>
-      <c r="AH40" s="4" t="n"/>
-      <c r="AI40" s="4" t="n"/>
-      <c r="AJ40" s="4" t="n"/>
-      <c r="AK40" s="4" t="n"/>
-      <c r="AL40" s="4" t="n"/>
-      <c r="AM40" s="4" t="n"/>
-      <c r="AN40" s="4" t="n"/>
-      <c r="AO40" s="4" t="n"/>
-      <c r="AP40" s="4" t="n"/>
-      <c r="AQ40" s="4" t="n"/>
-      <c r="AR40" s="4" t="n"/>
-      <c r="AS40" s="4" t="n"/>
-    </row>
   </sheetData>
-  <mergeCells count="35">
+  <mergeCells count="45">
     <mergeCell ref="AL25:AQ25"/>
     <mergeCell ref="AL26:AQ26"/>
     <mergeCell ref="AL27:AQ27"/>
@@ -2018,6 +2129,16 @@
     <mergeCell ref="X3:AC4"/>
     <mergeCell ref="AD3:AR4"/>
     <mergeCell ref="B4:W4"/>
+    <mergeCell ref="Y23:AB23"/>
+    <mergeCell ref="AC23:AE23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:X24"/>
+    <mergeCell ref="Y24:AB24"/>
+    <mergeCell ref="AC24:AE24"/>
+    <mergeCell ref="AF24:AJ24"/>
+    <mergeCell ref="AK24:AQ24"/>
+    <mergeCell ref="AL28:AQ28"/>
+    <mergeCell ref="AL29:AQ29"/>
   </mergeCells>
   <pageMargins left="0.75" right="1" top="0.75" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>